<commit_message>
CE09OSSM added barcodes where necessary
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE09OSSM_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_CE09OSSM_00002.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="29820" yWindow="1875" windowWidth="20730" windowHeight="11760" tabRatio="766" activeTab="1"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="263">
   <si>
     <t>Ref Des</t>
   </si>
@@ -459,33 +464,6 @@
     <t>CE09OSSM-MFD35-02-PRESFC000</t>
   </si>
   <si>
-    <t>CE09OSSM-00001-CPM1</t>
-  </si>
-  <si>
-    <t>CE09OSSM-00001-CPM2</t>
-  </si>
-  <si>
-    <t>CE09OSSM-00001-CPM3</t>
-  </si>
-  <si>
-    <t>CE09OSSM-00001-DCL11</t>
-  </si>
-  <si>
-    <t>CE09OSSM-00001-DCL12</t>
-  </si>
-  <si>
-    <t>CE09OSSM-00001-DCL26</t>
-  </si>
-  <si>
-    <t>CE09OSSM-00001-DCL27</t>
-  </si>
-  <si>
-    <t>CE09OSSM-00001-DCL35</t>
-  </si>
-  <si>
-    <t>CE09OSSM-00001-DCL37</t>
-  </si>
-  <si>
     <t>The serial number used here is bogus, pending identification of the real serial number.</t>
   </si>
   <si>
@@ -499,9 +477,6 @@
   </si>
   <si>
     <t>CE09OSSM-00002</t>
-  </si>
-  <si>
-    <t>6223-4220-43260</t>
   </si>
   <si>
     <t>35-257-50A</t>
@@ -675,13 +650,7 @@
     <t>CE09OSSM-00001</t>
   </si>
   <si>
-    <t>CE09OSSM-SBD11-HYDGN</t>
-  </si>
-  <si>
     <t>CE09OSSM-SBD12-03-HYDGN0000</t>
-  </si>
-  <si>
-    <t>CE09OSSM-SBD12-HYDGN</t>
   </si>
   <si>
     <t>Mooring OOIBARCODE</t>
@@ -784,6 +753,78 @@
   </si>
   <si>
     <t>CE09OSSM-MFD37-03-DOSTAD000</t>
+  </si>
+  <si>
+    <t>OL000457</t>
+  </si>
+  <si>
+    <t>OL000458</t>
+  </si>
+  <si>
+    <t>OL000459</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002+MOPAK</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-HYDGN11</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-HYDGN12</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-CPM1</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-CPM2</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-CPM3</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-DCL11</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-DCL12</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-DCL26</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-DCL27</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-DCL35</t>
+  </si>
+  <si>
+    <t>CE09OSSM-00002-DCL37</t>
+  </si>
+  <si>
+    <t>OL000463</t>
+  </si>
+  <si>
+    <t>OL000464</t>
+  </si>
+  <si>
+    <t>OL000465</t>
+  </si>
+  <si>
+    <t>OL000466</t>
+  </si>
+  <si>
+    <t>OL000467</t>
+  </si>
+  <si>
+    <t>OL000468</t>
+  </si>
+  <si>
+    <t>OL000460</t>
+  </si>
+  <si>
+    <t>OL000461</t>
+  </si>
+  <si>
+    <t>OL000462</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1324,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1408,6 +1449,7 @@
     <xf numFmtId="49" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="160">
     <cellStyle name="Comma 2" xfId="74"/>
@@ -1892,7 +1934,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1916,7 +1958,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -1954,13 +1996,13 @@
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -1975,16 +2017,16 @@
         <v>42497</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="J2" s="34">
         <v>542</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="35">
@@ -2026,8 +2068,8 @@
   <dimension ref="A1:M207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G139" sqref="G139"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2052,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>1</v>
@@ -2061,7 +2103,7 @@
         <v>34</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>2</v>
@@ -2089,19 +2131,19 @@
         <v>113</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D3" s="8">
         <v>2</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F3" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>5</v>
@@ -2110,7 +2152,7 @@
         <v>46.85313166666667</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2118,19 +2160,19 @@
         <v>113</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D4" s="8">
         <v>2</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>6</v>
@@ -2145,19 +2187,19 @@
         <v>113</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D5" s="8">
         <v>2</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>35</v>
@@ -2166,7 +2208,7 @@
         <v>1.35</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2174,19 +2216,19 @@
         <v>113</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D6" s="8">
         <v>2</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>36</v>
@@ -2195,7 +2237,7 @@
         <v>3.76</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2203,19 +2245,19 @@
         <v>113</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D7" s="8">
         <v>2</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>37</v>
@@ -2224,7 +2266,7 @@
         <v>3.76</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2232,19 +2274,19 @@
         <v>113</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D8" s="8">
         <v>2</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>38</v>
@@ -2253,7 +2295,7 @@
         <v>4.33</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2261,19 +2303,19 @@
         <v>113</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D9" s="8">
         <v>2</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>39</v>
@@ -2282,7 +2324,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2290,19 +2332,19 @@
         <v>113</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D10" s="8">
         <v>2</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F10" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>40</v>
@@ -2311,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2319,19 +2361,19 @@
         <v>113</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D11" s="8">
         <v>2</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>41</v>
@@ -2340,7 +2382,7 @@
         <v>600</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2348,19 +2390,22 @@
     </row>
     <row r="13" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D13" s="8">
         <v>2</v>
       </c>
-      <c r="F13" s="44" t="s">
-        <v>214</v>
+      <c r="E13" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2368,19 +2413,22 @@
     </row>
     <row r="15" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D15" s="8">
         <v>2</v>
       </c>
-      <c r="F15" s="44" t="s">
-        <v>216</v>
+      <c r="E15" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="F15" s="46" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2391,21 +2439,24 @@
         <v>112</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D17" s="8">
         <v>2</v>
       </c>
-      <c r="F17" s="45" t="s">
-        <v>156</v>
+      <c r="E17" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>242</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="22"/>
       <c r="I17" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2416,24 +2467,24 @@
         <v>136</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="F19" s="45" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="22"/>
       <c r="I19" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2444,19 +2495,19 @@
         <v>137</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>5</v>
@@ -2470,19 +2521,19 @@
         <v>137</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="F22" s="39" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>6</v>
@@ -2499,19 +2550,19 @@
         <v>114</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="F24" s="45" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
@@ -2525,19 +2576,19 @@
         <v>114</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="F25" s="45" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>6</v>
@@ -2554,16 +2605,16 @@
         <v>139</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D27" s="8">
         <v>2</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F27" s="45">
         <v>22717</v>
@@ -2575,7 +2626,7 @@
         <v>7000</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -2583,16 +2634,16 @@
         <v>139</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D28" s="8">
         <v>2</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F28" s="45">
         <v>22717</v>
@@ -2609,16 +2660,16 @@
         <v>139</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D29" s="8">
         <v>2</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F29" s="45">
         <v>22717</v>
@@ -2635,16 +2686,16 @@
         <v>139</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D30" s="8">
         <v>2</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F30" s="45">
         <v>22717</v>
@@ -2661,16 +2712,16 @@
         <v>139</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D31" s="8">
         <v>2</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F31" s="45">
         <v>22717</v>
@@ -2687,16 +2738,16 @@
         <v>139</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D32" s="8">
         <v>2</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F32" s="45">
         <v>22717</v>
@@ -2713,16 +2764,16 @@
         <v>139</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D33" s="8">
         <v>2</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F33" s="45">
         <v>22717</v>
@@ -2742,19 +2793,19 @@
         <v>121</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D35" s="8">
         <v>2</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F35" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>5</v>
@@ -2768,19 +2819,19 @@
         <v>121</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D36" s="8">
         <v>2</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F36" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>6</v>
@@ -2794,19 +2845,19 @@
         <v>121</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D37" s="8">
         <v>2</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F37" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>76</v>
@@ -2820,19 +2871,19 @@
         <v>121</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D38" s="8">
         <v>2</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F38" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>77</v>
@@ -2846,19 +2897,19 @@
         <v>121</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D39" s="8">
         <v>2</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F39" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>78</v>
@@ -2872,19 +2923,19 @@
         <v>121</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D40" s="8">
         <v>2</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F40" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>79</v>
@@ -2898,19 +2949,19 @@
         <v>121</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D41" s="8">
         <v>2</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F41" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>80</v>
@@ -2924,19 +2975,19 @@
         <v>121</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D42" s="8">
         <v>2</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F42" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>81</v>
@@ -2950,19 +3001,19 @@
         <v>121</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D43" s="8">
         <v>2</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F43" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>82</v>
@@ -2976,19 +3027,19 @@
         <v>121</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D44" s="8">
         <v>2</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F44" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>83</v>
@@ -3002,19 +3053,19 @@
         <v>121</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D45" s="8">
         <v>2</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F45" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>84</v>
@@ -3028,19 +3079,19 @@
         <v>121</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D46" s="8">
         <v>2</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F46" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>85</v>
@@ -3054,19 +3105,19 @@
         <v>121</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D47" s="8">
         <v>2</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F47" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>86</v>
@@ -3080,19 +3131,19 @@
         <v>121</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D48" s="8">
         <v>2</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F48" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>87</v>
@@ -3106,19 +3157,19 @@
         <v>121</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D49" s="8">
         <v>2</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F49" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>88</v>
@@ -3132,19 +3183,19 @@
         <v>121</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D50" s="8">
         <v>2</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F50" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>89</v>
@@ -3158,19 +3209,19 @@
         <v>121</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D51" s="8">
         <v>2</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F51" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>90</v>
@@ -3184,19 +3235,19 @@
         <v>121</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D52" s="8">
         <v>2</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F52" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>91</v>
@@ -3210,19 +3261,19 @@
         <v>121</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D53" s="8">
         <v>2</v>
       </c>
       <c r="E53" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F53" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>92</v>
@@ -3236,19 +3287,19 @@
         <v>121</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D54" s="8">
         <v>2</v>
       </c>
       <c r="E54" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F54" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>93</v>
@@ -3262,19 +3313,19 @@
         <v>121</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D55" s="8">
         <v>2</v>
       </c>
       <c r="E55" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F55" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>94</v>
@@ -3288,19 +3339,19 @@
         <v>121</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D56" s="8">
         <v>2</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F56" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>95</v>
@@ -3314,19 +3365,19 @@
         <v>121</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D57" s="8">
         <v>2</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F57" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>96</v>
@@ -3340,19 +3391,19 @@
         <v>121</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D58" s="8">
         <v>2</v>
       </c>
       <c r="E58" s="26" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F58" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>97</v>
@@ -3369,16 +3420,16 @@
         <v>122</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D60" s="8">
         <v>2</v>
       </c>
       <c r="E60" s="26" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="F60" s="45">
         <v>219</v>
@@ -3395,16 +3446,16 @@
         <v>122</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D61" s="8">
         <v>2</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="F61" s="45">
         <v>219</v>
@@ -3421,16 +3472,16 @@
         <v>122</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D62" s="8">
         <v>2</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="F62" s="45">
         <v>219</v>
@@ -3439,7 +3490,7 @@
         <v>11</v>
       </c>
       <c r="H62" s="22" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3447,28 +3498,28 @@
         <v>122</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D63" s="8">
         <v>2</v>
       </c>
       <c r="E63" s="26" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="F63" s="45">
         <v>219</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H63" s="22" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3480,16 +3531,16 @@
         <v>120</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D65" s="8">
         <v>2</v>
       </c>
       <c r="E65" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F65" s="45">
         <v>1291</v>
@@ -3506,16 +3557,16 @@
         <v>120</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D66" s="8">
         <v>2</v>
       </c>
       <c r="E66" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F66" s="45">
         <v>1291</v>
@@ -3532,16 +3583,16 @@
         <v>120</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D67" s="8">
         <v>2</v>
       </c>
       <c r="E67" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F67" s="45">
         <v>1291</v>
@@ -3558,16 +3609,16 @@
         <v>120</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D68" s="8">
         <v>2</v>
       </c>
       <c r="E68" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F68" s="45">
         <v>1291</v>
@@ -3584,16 +3635,16 @@
         <v>120</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D69" s="8">
         <v>2</v>
       </c>
       <c r="E69" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F69" s="45">
         <v>1291</v>
@@ -3610,16 +3661,16 @@
         <v>120</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D70" s="8">
         <v>2</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F70" s="45">
         <v>1291</v>
@@ -3636,16 +3687,16 @@
         <v>120</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D71" s="8">
         <v>2</v>
       </c>
       <c r="E71" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F71" s="45">
         <v>1291</v>
@@ -3657,7 +3708,7 @@
         <v>124</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3665,16 +3716,16 @@
         <v>120</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D72" s="8">
         <v>2</v>
       </c>
       <c r="E72" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F72" s="45">
         <v>1291</v>
@@ -3694,16 +3745,16 @@
         <v>120</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D73" s="8">
         <v>2</v>
       </c>
       <c r="E73" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F73" s="45">
         <v>1291</v>
@@ -3715,7 +3766,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3723,16 +3774,16 @@
         <v>120</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D74" s="8">
         <v>2</v>
       </c>
       <c r="E74" s="26" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F74" s="45">
         <v>1291</v>
@@ -3756,16 +3807,16 @@
         <v>123</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D76" s="8">
         <v>2</v>
       </c>
       <c r="E76" s="26" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F76" s="45">
         <v>254</v>
@@ -3785,16 +3836,16 @@
         <v>123</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D77" s="8">
         <v>2</v>
       </c>
       <c r="E77" s="26" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F77" s="45">
         <v>254</v>
@@ -3814,16 +3865,16 @@
         <v>123</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D78" s="8">
         <v>2</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F78" s="45">
         <v>254</v>
@@ -3840,16 +3891,16 @@
         <v>123</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D79" s="8">
         <v>2</v>
       </c>
       <c r="E79" s="26" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F79" s="45">
         <v>254</v>
@@ -3858,7 +3909,7 @@
         <v>47</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3866,16 +3917,16 @@
         <v>123</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D80" s="8">
         <v>2</v>
       </c>
       <c r="E80" s="26" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F80" s="45">
         <v>254</v>
@@ -3884,7 +3935,7 @@
         <v>48</v>
       </c>
       <c r="H80" s="22" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3892,16 +3943,16 @@
         <v>123</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D81" s="8">
         <v>2</v>
       </c>
       <c r="E81" s="26" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F81" s="45">
         <v>254</v>
@@ -3910,7 +3961,7 @@
         <v>49</v>
       </c>
       <c r="H81" s="22" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3918,16 +3969,16 @@
         <v>123</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D82" s="8">
         <v>2</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F82" s="45">
         <v>254</v>
@@ -3936,10 +3987,10 @@
         <v>50</v>
       </c>
       <c r="H82" s="22" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3950,25 +4001,25 @@
         <v>118</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D84" s="8">
         <v>2</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F84" s="39" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G84" s="8" t="s">
         <v>101</v>
       </c>
       <c r="H84" s="22" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3976,25 +4027,25 @@
         <v>118</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D85" s="8">
         <v>2</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F85" s="39" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G85" s="8" t="s">
         <v>102</v>
       </c>
       <c r="H85" s="22" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4002,19 +4053,19 @@
         <v>118</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D86" s="8">
         <v>2</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F86" s="39" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G86" s="8" t="s">
         <v>42</v>
@@ -4028,25 +4079,25 @@
         <v>118</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D87" s="8">
         <v>2</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F87" s="39" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G87" s="8" t="s">
         <v>43</v>
       </c>
       <c r="H87" s="22" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4054,25 +4105,25 @@
         <v>118</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D88" s="8">
         <v>2</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F88" s="39" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G88" s="8" t="s">
         <v>103</v>
       </c>
       <c r="H88" s="22" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4080,25 +4131,25 @@
         <v>118</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D89" s="8">
         <v>2</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F89" s="39" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G89" s="8" t="s">
         <v>104</v>
       </c>
       <c r="H89" s="22" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4106,25 +4157,25 @@
         <v>118</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D90" s="8">
         <v>2</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F90" s="39" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G90" s="8" t="s">
         <v>105</v>
       </c>
       <c r="H90" s="22" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4132,25 +4183,25 @@
         <v>118</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D91" s="8">
         <v>2</v>
       </c>
       <c r="E91" s="26" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="F91" s="39" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>106</v>
       </c>
       <c r="H91" s="25" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4161,19 +4212,19 @@
         <v>116</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D93" s="1">
         <v>2</v>
       </c>
       <c r="E93" s="26" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F93" s="45" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G93" s="8" t="s">
         <v>14</v>
@@ -4187,19 +4238,19 @@
         <v>116</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D94" s="8">
         <v>2</v>
       </c>
       <c r="E94" s="26" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F94" s="45" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G94" s="8" t="s">
         <v>16</v>
@@ -4213,19 +4264,19 @@
         <v>116</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D95" s="8">
         <v>2</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F95" s="45" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G95" s="8" t="s">
         <v>15</v>
@@ -4239,19 +4290,19 @@
         <v>116</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D96" s="8">
         <v>2</v>
       </c>
       <c r="E96" s="26" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F96" s="45" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G96" s="8" t="s">
         <v>17</v>
@@ -4265,19 +4316,19 @@
         <v>116</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D97" s="8">
         <v>2</v>
       </c>
       <c r="E97" s="26" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F97" s="45" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>19</v>
@@ -4286,7 +4337,7 @@
         <v>0</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4294,19 +4345,19 @@
         <v>116</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D98" s="8">
         <v>2</v>
       </c>
       <c r="E98" s="26" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F98" s="45" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G98" s="8" t="s">
         <v>18</v>
@@ -4315,7 +4366,7 @@
         <v>1</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4323,19 +4374,19 @@
         <v>116</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D99" s="8">
         <v>2</v>
       </c>
       <c r="E99" s="26" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F99" s="43" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G99" s="8" t="s">
         <v>100</v>
@@ -4344,7 +4395,7 @@
         <v>35</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4355,16 +4406,16 @@
         <v>124</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D101" s="8">
         <v>2</v>
       </c>
       <c r="E101" s="26" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="F101" s="45">
         <v>254</v>
@@ -4373,7 +4424,7 @@
         <v>51</v>
       </c>
       <c r="H101" s="27" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4381,16 +4432,16 @@
         <v>124</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D102" s="8">
         <v>2</v>
       </c>
       <c r="E102" s="26" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="F102" s="45">
         <v>254</v>
@@ -4399,7 +4450,7 @@
         <v>52</v>
       </c>
       <c r="H102" s="27" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4407,16 +4458,16 @@
         <v>124</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D103" s="8">
         <v>2</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="F103" s="45">
         <v>254</v>
@@ -4425,7 +4476,7 @@
         <v>53</v>
       </c>
       <c r="H103" s="27" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4437,19 +4488,19 @@
         <v>115</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D105" s="1">
         <v>2</v>
       </c>
       <c r="E105" s="26" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="F105" s="39" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="G105" s="8" t="s">
         <v>5</v>
@@ -4463,19 +4514,19 @@
         <v>115</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D106" s="1">
         <v>2</v>
       </c>
       <c r="E106" s="26" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="F106" s="39" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="G106" s="8" t="s">
         <v>6</v>
@@ -4492,16 +4543,16 @@
         <v>140</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D108" s="8">
         <v>2</v>
       </c>
       <c r="E108" s="26" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F108" s="45">
         <v>22649</v>
@@ -4513,7 +4564,7 @@
         <v>542000</v>
       </c>
       <c r="I108" s="22" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4521,16 +4572,16 @@
         <v>140</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D109" s="8">
         <v>2</v>
       </c>
       <c r="E109" s="26" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F109" s="45">
         <v>22649</v>
@@ -4547,16 +4598,16 @@
         <v>140</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D110" s="8">
         <v>2</v>
       </c>
       <c r="E110" s="26" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F110" s="45">
         <v>22649</v>
@@ -4573,16 +4624,16 @@
         <v>140</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D111" s="8">
         <v>2</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F111" s="45">
         <v>22649</v>
@@ -4599,16 +4650,16 @@
         <v>140</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D112" s="8">
         <v>2</v>
       </c>
       <c r="E112" s="26" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F112" s="45">
         <v>22649</v>
@@ -4625,16 +4676,16 @@
         <v>140</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D113" s="8">
         <v>2</v>
       </c>
       <c r="E113" s="26" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F113" s="45">
         <v>22649</v>
@@ -4651,16 +4702,16 @@
         <v>140</v>
       </c>
       <c r="B114" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D114" s="8">
         <v>2</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F114" s="45">
         <v>22649</v>
@@ -4681,19 +4732,19 @@
     <row r="116" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F116" s="43"/>
       <c r="I116" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="J116" s="8" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="K116" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="L116" s="8">
         <v>2</v>
       </c>
       <c r="M116" s="23" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4704,19 +4755,19 @@
         <v>138</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D118" s="8">
         <v>2</v>
       </c>
       <c r="E118" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F118" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G118" s="8" t="s">
         <v>5</v>
@@ -4730,19 +4781,19 @@
         <v>138</v>
       </c>
       <c r="B119" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D119" s="8">
         <v>2</v>
       </c>
       <c r="E119" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F119" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G119" s="8" t="s">
         <v>6</v>
@@ -4756,19 +4807,19 @@
         <v>138</v>
       </c>
       <c r="B120" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D120" s="8">
         <v>2</v>
       </c>
       <c r="E120" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F120" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G120" s="8" t="s">
         <v>76</v>
@@ -4782,19 +4833,19 @@
         <v>138</v>
       </c>
       <c r="B121" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D121" s="8">
         <v>2</v>
       </c>
       <c r="E121" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F121" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G121" s="8" t="s">
         <v>77</v>
@@ -4808,19 +4859,19 @@
         <v>138</v>
       </c>
       <c r="B122" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D122" s="8">
         <v>2</v>
       </c>
       <c r="E122" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F122" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G122" s="8" t="s">
         <v>78</v>
@@ -4834,19 +4885,19 @@
         <v>138</v>
       </c>
       <c r="B123" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D123" s="8">
         <v>2</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F123" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G123" s="8" t="s">
         <v>79</v>
@@ -4860,19 +4911,19 @@
         <v>138</v>
       </c>
       <c r="B124" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D124" s="8">
         <v>2</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F124" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G124" s="8" t="s">
         <v>80</v>
@@ -4886,19 +4937,19 @@
         <v>138</v>
       </c>
       <c r="B125" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D125" s="8">
         <v>2</v>
       </c>
       <c r="E125" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F125" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G125" s="8" t="s">
         <v>81</v>
@@ -4912,19 +4963,19 @@
         <v>138</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D126" s="8">
         <v>2</v>
       </c>
       <c r="E126" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F126" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G126" s="8" t="s">
         <v>82</v>
@@ -4938,19 +4989,19 @@
         <v>138</v>
       </c>
       <c r="B127" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D127" s="8">
         <v>2</v>
       </c>
       <c r="E127" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F127" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G127" s="8" t="s">
         <v>83</v>
@@ -4964,19 +5015,19 @@
         <v>138</v>
       </c>
       <c r="B128" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D128" s="8">
         <v>2</v>
       </c>
       <c r="E128" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F128" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G128" s="8" t="s">
         <v>84</v>
@@ -4990,19 +5041,19 @@
         <v>138</v>
       </c>
       <c r="B129" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D129" s="8">
         <v>2</v>
       </c>
       <c r="E129" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F129" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G129" s="8" t="s">
         <v>85</v>
@@ -5016,19 +5067,19 @@
         <v>138</v>
       </c>
       <c r="B130" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D130" s="8">
         <v>2</v>
       </c>
       <c r="E130" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F130" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G130" s="8" t="s">
         <v>86</v>
@@ -5042,19 +5093,19 @@
         <v>138</v>
       </c>
       <c r="B131" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D131" s="8">
         <v>2</v>
       </c>
       <c r="E131" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F131" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G131" s="8" t="s">
         <v>87</v>
@@ -5063,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="I131" s="8" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="132" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -5071,19 +5122,19 @@
         <v>138</v>
       </c>
       <c r="B132" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D132" s="8">
         <v>2</v>
       </c>
       <c r="E132" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F132" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G132" s="8" t="s">
         <v>88</v>
@@ -5097,19 +5148,19 @@
         <v>138</v>
       </c>
       <c r="B133" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D133" s="8">
         <v>2</v>
       </c>
       <c r="E133" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F133" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G133" s="8" t="s">
         <v>89</v>
@@ -5123,19 +5174,19 @@
         <v>138</v>
       </c>
       <c r="B134" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D134" s="8">
         <v>2</v>
       </c>
       <c r="E134" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F134" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G134" s="8" t="s">
         <v>90</v>
@@ -5149,19 +5200,19 @@
         <v>138</v>
       </c>
       <c r="B135" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D135" s="8">
         <v>2</v>
       </c>
       <c r="E135" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F135" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G135" s="8" t="s">
         <v>91</v>
@@ -5175,19 +5226,19 @@
         <v>138</v>
       </c>
       <c r="B136" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D136" s="8">
         <v>2</v>
       </c>
       <c r="E136" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F136" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G136" s="8" t="s">
         <v>92</v>
@@ -5201,19 +5252,19 @@
         <v>138</v>
       </c>
       <c r="B137" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D137" s="8">
         <v>2</v>
       </c>
       <c r="E137" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F137" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G137" s="8" t="s">
         <v>93</v>
@@ -5227,19 +5278,19 @@
         <v>138</v>
       </c>
       <c r="B138" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D138" s="8">
         <v>2</v>
       </c>
       <c r="E138" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F138" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G138" s="8" t="s">
         <v>94</v>
@@ -5253,19 +5304,19 @@
         <v>138</v>
       </c>
       <c r="B139" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D139" s="8">
         <v>2</v>
       </c>
       <c r="E139" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F139" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G139" s="8" t="s">
         <v>95</v>
@@ -5279,19 +5330,19 @@
         <v>138</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D140" s="8">
         <v>2</v>
       </c>
       <c r="E140" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F140" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G140" s="8" t="s">
         <v>96</v>
@@ -5305,19 +5356,19 @@
         <v>138</v>
       </c>
       <c r="B141" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D141" s="8">
         <v>2</v>
       </c>
       <c r="E141" s="26" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F141" s="45" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G141" s="8" t="s">
         <v>97</v>
@@ -5332,19 +5383,19 @@
     </row>
     <row r="143" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B143" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D143" s="8">
         <v>2</v>
       </c>
       <c r="E143" s="26" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="F143" s="45">
         <v>478</v>
@@ -5358,19 +5409,19 @@
     </row>
     <row r="144" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B144" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D144" s="8">
         <v>2</v>
       </c>
       <c r="E144" s="26" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="F144" s="45">
         <v>478</v>
@@ -5384,19 +5435,19 @@
     </row>
     <row r="145" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B145" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D145" s="8">
         <v>2</v>
       </c>
       <c r="E145" s="26" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="F145" s="45">
         <v>478</v>
@@ -5405,36 +5456,36 @@
         <v>11</v>
       </c>
       <c r="H145" s="22" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="146" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B146" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D146" s="8">
         <v>2</v>
       </c>
       <c r="E146" s="26" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="F146" s="45">
         <v>478</v>
       </c>
       <c r="G146" s="8" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H146" s="22" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="I146" s="8" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5446,25 +5497,25 @@
         <v>119</v>
       </c>
       <c r="B148" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D148" s="8">
         <v>2</v>
       </c>
       <c r="E148" s="26" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F148" s="39" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G148" s="8" t="s">
         <v>101</v>
       </c>
       <c r="H148" s="27" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -5472,25 +5523,25 @@
         <v>119</v>
       </c>
       <c r="B149" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D149" s="8">
         <v>2</v>
       </c>
       <c r="E149" s="26" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F149" s="39" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G149" s="8" t="s">
         <v>102</v>
       </c>
       <c r="H149" s="27" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -5498,19 +5549,19 @@
         <v>119</v>
       </c>
       <c r="B150" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D150" s="8">
         <v>2</v>
       </c>
       <c r="E150" s="26" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F150" s="39" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G150" s="8" t="s">
         <v>42</v>
@@ -5524,25 +5575,25 @@
         <v>119</v>
       </c>
       <c r="B151" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D151" s="8">
         <v>2</v>
       </c>
       <c r="E151" s="26" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F151" s="39" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G151" s="8" t="s">
         <v>43</v>
       </c>
       <c r="H151" s="27" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -5550,25 +5601,25 @@
         <v>119</v>
       </c>
       <c r="B152" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D152" s="8">
         <v>2</v>
       </c>
       <c r="E152" s="26" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F152" s="39" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G152" s="8" t="s">
         <v>103</v>
       </c>
       <c r="H152" s="27" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -5576,25 +5627,25 @@
         <v>119</v>
       </c>
       <c r="B153" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D153" s="8">
         <v>2</v>
       </c>
       <c r="E153" s="26" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F153" s="39" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G153" s="8" t="s">
         <v>104</v>
       </c>
       <c r="H153" s="27" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -5602,25 +5653,25 @@
         <v>119</v>
       </c>
       <c r="B154" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D154" s="8">
         <v>2</v>
       </c>
       <c r="E154" s="26" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F154" s="39" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G154" s="8" t="s">
         <v>105</v>
       </c>
       <c r="H154" s="27" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -5628,25 +5679,25 @@
         <v>119</v>
       </c>
       <c r="B155" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D155" s="8">
         <v>2</v>
       </c>
       <c r="E155" s="26" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F155" s="39" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G155" s="8" t="s">
         <v>106</v>
       </c>
       <c r="H155" s="27" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -5658,19 +5709,19 @@
         <v>126</v>
       </c>
       <c r="B157" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D157" s="8">
         <v>2</v>
       </c>
       <c r="E157" s="26" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F157" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>70</v>
@@ -5684,19 +5735,19 @@
         <v>126</v>
       </c>
       <c r="B158" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D158" s="8">
         <v>2</v>
       </c>
       <c r="E158" s="26" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F158" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>71</v>
@@ -5710,19 +5761,19 @@
         <v>126</v>
       </c>
       <c r="B159" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D159" s="8">
         <v>2</v>
       </c>
       <c r="E159" s="26" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F159" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G159" s="1" t="s">
         <v>72</v>
@@ -5736,19 +5787,19 @@
         <v>126</v>
       </c>
       <c r="B160" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D160" s="8">
         <v>2</v>
       </c>
       <c r="E160" s="26" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F160" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>73</v>
@@ -5762,19 +5813,19 @@
         <v>126</v>
       </c>
       <c r="B161" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D161" s="8">
         <v>2</v>
       </c>
       <c r="E161" s="26" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F161" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G161" s="1" t="s">
         <v>14</v>
@@ -5783,7 +5834,7 @@
         <v>19706</v>
       </c>
       <c r="I161" s="30" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -5791,19 +5842,19 @@
         <v>126</v>
       </c>
       <c r="B162" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D162" s="8">
         <v>2</v>
       </c>
       <c r="E162" s="26" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F162" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G162" s="1" t="s">
         <v>74</v>
@@ -5812,7 +5863,7 @@
         <v>34</v>
       </c>
       <c r="I162" s="31" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -5820,19 +5871,19 @@
         <v>126</v>
       </c>
       <c r="B163" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D163" s="8">
         <v>2</v>
       </c>
       <c r="E163" s="26" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F163" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G163" s="1" t="s">
         <v>15</v>
@@ -5847,19 +5898,19 @@
         <v>126</v>
       </c>
       <c r="B164" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D164" s="8">
         <v>2</v>
       </c>
       <c r="E164" s="26" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F164" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>75</v>
@@ -5877,19 +5928,19 @@
         <v>117</v>
       </c>
       <c r="B166" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D166" s="8">
         <v>2</v>
       </c>
       <c r="E166" s="26" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="F166" s="45" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G166" s="8" t="s">
         <v>14</v>
@@ -5903,19 +5954,19 @@
         <v>117</v>
       </c>
       <c r="B167" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D167" s="8">
         <v>2</v>
       </c>
       <c r="E167" s="26" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="F167" s="45" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G167" s="8" t="s">
         <v>16</v>
@@ -5929,19 +5980,19 @@
         <v>117</v>
       </c>
       <c r="B168" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D168" s="8">
         <v>2</v>
       </c>
       <c r="E168" s="26" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="F168" s="45" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G168" s="8" t="s">
         <v>15</v>
@@ -5955,19 +6006,19 @@
         <v>117</v>
       </c>
       <c r="B169" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D169" s="8">
         <v>2</v>
       </c>
       <c r="E169" s="26" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="F169" s="45" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G169" s="8" t="s">
         <v>17</v>
@@ -5981,19 +6032,19 @@
         <v>117</v>
       </c>
       <c r="B170" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D170" s="8">
         <v>2</v>
       </c>
       <c r="E170" s="26" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="F170" s="45" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G170" s="8" t="s">
         <v>19</v>
@@ -6002,7 +6053,7 @@
         <v>0</v>
       </c>
       <c r="I170" s="8" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6010,19 +6061,19 @@
         <v>117</v>
       </c>
       <c r="B171" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D171" s="8">
         <v>2</v>
       </c>
       <c r="E171" s="26" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="F171" s="45" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G171" s="8" t="s">
         <v>18</v>
@@ -6031,7 +6082,7 @@
         <v>1</v>
       </c>
       <c r="I171" s="8" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6039,19 +6090,19 @@
         <v>117</v>
       </c>
       <c r="B172" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D172" s="8">
         <v>2</v>
       </c>
       <c r="E172" s="26" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="F172" s="43" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G172" s="8" t="s">
         <v>100</v>
@@ -6060,7 +6111,7 @@
         <v>35</v>
       </c>
       <c r="I172" s="8" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -6071,19 +6122,19 @@
         <v>141</v>
       </c>
       <c r="B174" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D174" s="8">
         <v>2</v>
       </c>
       <c r="E174" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F174" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>56</v>
@@ -6092,7 +6143,7 @@
         <v>-4631.5259999999998</v>
       </c>
       <c r="I174" s="8" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6100,19 +6151,19 @@
         <v>141</v>
       </c>
       <c r="B175" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D175" s="8">
         <v>2</v>
       </c>
       <c r="E175" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F175" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>57</v>
@@ -6121,7 +6172,7 @@
         <v>35.767060000000001</v>
       </c>
       <c r="I175" s="8" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6129,19 +6180,19 @@
         <v>141</v>
       </c>
       <c r="B176" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D176" s="8">
         <v>2</v>
       </c>
       <c r="E176" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F176" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G176" s="1" t="s">
         <v>58</v>
@@ -6155,19 +6206,19 @@
         <v>141</v>
       </c>
       <c r="B177" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D177" s="8">
         <v>2</v>
       </c>
       <c r="E177" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F177" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G177" s="1" t="s">
         <v>59</v>
@@ -6181,19 +6232,19 @@
         <v>141</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D178" s="8">
         <v>2</v>
       </c>
       <c r="E178" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F178" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G178" s="1" t="s">
         <v>60</v>
@@ -6207,19 +6258,19 @@
         <v>141</v>
       </c>
       <c r="B179" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D179" s="8">
         <v>2</v>
       </c>
       <c r="E179" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F179" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G179" s="1" t="s">
         <v>54</v>
@@ -6236,19 +6287,19 @@
         <v>141</v>
       </c>
       <c r="B180" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D180" s="8">
         <v>2</v>
       </c>
       <c r="E180" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F180" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G180" s="1" t="s">
         <v>61</v>
@@ -6257,7 +6308,7 @@
         <v>-0.38400000000000001</v>
       </c>
       <c r="I180" s="33" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6265,19 +6316,19 @@
         <v>141</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D181" s="8">
         <v>2</v>
       </c>
       <c r="E181" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F181" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>55</v>
@@ -6294,19 +6345,19 @@
         <v>141</v>
       </c>
       <c r="B182" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D182" s="8">
         <v>2</v>
       </c>
       <c r="E182" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F182" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G182" s="1" t="s">
         <v>62</v>
@@ -6320,19 +6371,19 @@
         <v>141</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D183" s="8">
         <v>2</v>
       </c>
       <c r="E183" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F183" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G183" s="1" t="s">
         <v>63</v>
@@ -6346,19 +6397,19 @@
         <v>141</v>
       </c>
       <c r="B184" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D184" s="8">
         <v>2</v>
       </c>
       <c r="E184" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F184" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G184" s="1" t="s">
         <v>64</v>
@@ -6372,19 +6423,19 @@
         <v>141</v>
       </c>
       <c r="B185" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D185" s="8">
         <v>2</v>
       </c>
       <c r="E185" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F185" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>65</v>
@@ -6398,19 +6449,19 @@
         <v>141</v>
       </c>
       <c r="B186" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D186" s="8">
         <v>2</v>
       </c>
       <c r="E186" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F186" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G186" s="1" t="s">
         <v>66</v>
@@ -6424,19 +6475,19 @@
         <v>141</v>
       </c>
       <c r="B187" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D187" s="8">
         <v>2</v>
       </c>
       <c r="E187" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F187" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G187" s="1" t="s">
         <v>67</v>
@@ -6450,19 +6501,19 @@
         <v>141</v>
       </c>
       <c r="B188" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D188" s="8">
         <v>2</v>
       </c>
       <c r="E188" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F188" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G188" s="1" t="s">
         <v>68</v>
@@ -6476,19 +6527,19 @@
         <v>141</v>
       </c>
       <c r="B189" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D189" s="8">
         <v>2</v>
       </c>
       <c r="E189" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F189" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>69</v>
@@ -6502,19 +6553,19 @@
         <v>141</v>
       </c>
       <c r="B190" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D190" s="8">
         <v>2</v>
       </c>
       <c r="E190" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F190" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G190" s="8" t="s">
         <v>98</v>
@@ -6528,19 +6579,19 @@
         <v>141</v>
       </c>
       <c r="B191" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D191" s="8">
         <v>2</v>
       </c>
       <c r="E191" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F191" s="39" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G191" s="8" t="s">
         <v>99</v>
@@ -6557,16 +6608,16 @@
         <v>125</v>
       </c>
       <c r="B193" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D193" s="8">
         <v>2</v>
       </c>
       <c r="E193" s="26" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="F193" s="45">
         <v>12607</v>
@@ -6583,16 +6634,16 @@
         <v>125</v>
       </c>
       <c r="B194" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D194" s="8">
         <v>2</v>
       </c>
       <c r="E194" s="26" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="F194" s="45">
         <v>12607</v>
@@ -6613,26 +6664,26 @@
     </row>
     <row r="196" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="8" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B196" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D196" s="8">
         <v>2</v>
       </c>
       <c r="E196" s="26" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="F196" s="45">
         <v>55096</v>
       </c>
       <c r="H196" s="22"/>
       <c r="I196" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="197" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -6643,19 +6694,22 @@
         <v>127</v>
       </c>
       <c r="B198" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D198" s="8">
         <v>2</v>
       </c>
-      <c r="F198" s="44" t="s">
+      <c r="E198" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="F198" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="I198" s="19" t="s">
         <v>142</v>
-      </c>
-      <c r="I198" s="19" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="199" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6663,19 +6717,22 @@
         <v>128</v>
       </c>
       <c r="B199" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D199" s="8">
         <v>2</v>
       </c>
-      <c r="F199" s="44" t="s">
-        <v>143</v>
+      <c r="E199" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="F199" s="8" t="s">
+        <v>246</v>
       </c>
       <c r="I199" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="200" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6683,19 +6740,22 @@
         <v>129</v>
       </c>
       <c r="B200" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D200" s="8">
         <v>2</v>
       </c>
-      <c r="F200" s="44" t="s">
-        <v>144</v>
+      <c r="E200" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="F200" s="8" t="s">
+        <v>247</v>
       </c>
       <c r="I200" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -6708,19 +6768,22 @@
         <v>130</v>
       </c>
       <c r="B202" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D202" s="8">
         <v>2</v>
       </c>
-      <c r="F202" s="44" t="s">
-        <v>145</v>
+      <c r="E202" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="F202" s="8" t="s">
+        <v>248</v>
       </c>
       <c r="I202" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="203" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6728,19 +6791,22 @@
         <v>131</v>
       </c>
       <c r="B203" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D203" s="8">
         <v>2</v>
       </c>
-      <c r="F203" s="44" t="s">
-        <v>146</v>
+      <c r="E203" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="F203" s="8" t="s">
+        <v>249</v>
       </c>
       <c r="I203" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="204" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6748,19 +6814,22 @@
         <v>132</v>
       </c>
       <c r="B204" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D204" s="8">
         <v>2</v>
       </c>
-      <c r="F204" s="44" t="s">
-        <v>147</v>
+      <c r="E204" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="F204" s="8" t="s">
+        <v>250</v>
       </c>
       <c r="I204" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="205" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6768,19 +6837,22 @@
         <v>133</v>
       </c>
       <c r="B205" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D205" s="8">
         <v>2</v>
       </c>
-      <c r="F205" s="44" t="s">
-        <v>148</v>
+      <c r="E205" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="F205" s="8" t="s">
+        <v>251</v>
       </c>
       <c r="I205" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="206" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6788,19 +6860,22 @@
         <v>134</v>
       </c>
       <c r="B206" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D206" s="8">
         <v>2</v>
       </c>
-      <c r="F206" s="44" t="s">
-        <v>149</v>
+      <c r="E206" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="F206" s="8" t="s">
+        <v>252</v>
       </c>
       <c r="I206" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="207" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -6808,19 +6883,22 @@
         <v>135</v>
       </c>
       <c r="B207" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D207" s="8">
         <v>2</v>
       </c>
-      <c r="F207" s="44" t="s">
-        <v>150</v>
+      <c r="E207" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="F207" s="8" t="s">
+        <v>253</v>
       </c>
       <c r="I207" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>